<commit_message>
updated hand_landmark_estimation.py and merging by User3198352
</commit_message>
<xml_diff>
--- a/Mergy_Hand_Pose_Estimation_Preprocessing/landmarks.xlsx
+++ b/Mergy_Hand_Pose_Estimation_Preprocessing/landmarks.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,10 +443,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>454.6867752075195</v>
+        <v>321.9075393676758</v>
       </c>
       <c r="C2" t="n">
-        <v>130.6136512756348</v>
+        <v>156.5245199203491</v>
       </c>
     </row>
     <row r="3">
@@ -454,10 +454,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>453.3409881591797</v>
+        <v>321.1606979370117</v>
       </c>
       <c r="C3" t="n">
-        <v>131.1065483093262</v>
+        <v>156.6767406463623</v>
       </c>
     </row>
     <row r="4">
@@ -465,10 +465,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>453.9939117431641</v>
+        <v>320.3333282470703</v>
       </c>
       <c r="C4" t="n">
-        <v>133.5875701904297</v>
+        <v>156.4820194244385</v>
       </c>
     </row>
     <row r="5">
@@ -476,10 +476,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>454.182014465332</v>
+        <v>320.5591583251953</v>
       </c>
       <c r="C5" t="n">
-        <v>136.8184089660645</v>
+        <v>157.2189903259277</v>
       </c>
     </row>
     <row r="6">
@@ -487,10 +487,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>454.2490386962891</v>
+        <v>320.1755523681641</v>
       </c>
       <c r="C6" t="n">
-        <v>138.1896114349365</v>
+        <v>157.4060726165771</v>
       </c>
     </row>
     <row r="7">
@@ -498,10 +498,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>455.6053161621094</v>
+        <v>320.0727081298828</v>
       </c>
       <c r="C7" t="n">
-        <v>140.6483602523804</v>
+        <v>157.2195911407471</v>
       </c>
     </row>
     <row r="8">
@@ -509,10 +509,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>455.8718490600586</v>
+        <v>320.9890747070312</v>
       </c>
       <c r="C8" t="n">
-        <v>142.5516700744629</v>
+        <v>157.6928758621216</v>
       </c>
     </row>
     <row r="9">
@@ -520,10 +520,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>457.7560043334961</v>
+        <v>322.1222686767578</v>
       </c>
       <c r="C9" t="n">
-        <v>144.0362691879272</v>
+        <v>158.0412340164185</v>
       </c>
     </row>
     <row r="10">
@@ -531,10 +531,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>458.3106994628906</v>
+        <v>324.2362976074219</v>
       </c>
       <c r="C10" t="n">
-        <v>142.9345321655273</v>
+        <v>158.3535003662109</v>
       </c>
     </row>
     <row r="11">
@@ -542,10 +542,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>456.0019302368164</v>
+        <v>324.840087890625</v>
       </c>
       <c r="C11" t="n">
-        <v>138.7496852874756</v>
+        <v>157.8266572952271</v>
       </c>
     </row>
     <row r="12">
@@ -553,10 +553,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>448.2406997680664</v>
+        <v>325.7466125488281</v>
       </c>
       <c r="C12" t="n">
-        <v>129.3004417419434</v>
+        <v>157.1883773803711</v>
       </c>
     </row>
     <row r="13">
@@ -564,10 +564,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>433.7151718139648</v>
+        <v>325.0298309326172</v>
       </c>
       <c r="C13" t="n">
-        <v>114.4113421440125</v>
+        <v>156.2177610397339</v>
       </c>
     </row>
     <row r="14">
@@ -575,10 +575,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>413.5909271240234</v>
+        <v>321.9512176513672</v>
       </c>
       <c r="C14" t="n">
-        <v>98.37455034255981</v>
+        <v>154.4462299346924</v>
       </c>
     </row>
     <row r="15">
@@ -586,10 +586,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>389.4297790527344</v>
+        <v>317.0373725891113</v>
       </c>
       <c r="C15" t="n">
-        <v>88.38284969329834</v>
+        <v>149.9756526947021</v>
       </c>
     </row>
     <row r="16">
@@ -597,10 +597,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>362.9389953613281</v>
+        <v>308.841438293457</v>
       </c>
       <c r="C16" t="n">
-        <v>80.71746826171875</v>
+        <v>144.9496078491211</v>
       </c>
     </row>
     <row r="17">
@@ -608,10 +608,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>336.7771530151367</v>
+        <v>296.7984390258789</v>
       </c>
       <c r="C17" t="n">
-        <v>78.18661451339722</v>
+        <v>138.9054107666016</v>
       </c>
     </row>
     <row r="18">
@@ -619,10 +619,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>312.2503852844238</v>
+        <v>283.856201171875</v>
       </c>
       <c r="C18" t="n">
-        <v>84.61982488632202</v>
+        <v>133.2048225402832</v>
       </c>
     </row>
     <row r="19">
@@ -630,10 +630,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>290.5868148803711</v>
+        <v>268.5635757446289</v>
       </c>
       <c r="C19" t="n">
-        <v>95.0274395942688</v>
+        <v>127.4671411514282</v>
       </c>
     </row>
     <row r="20">
@@ -641,10 +641,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>271.4570426940918</v>
+        <v>253.7520217895508</v>
       </c>
       <c r="C20" t="n">
-        <v>110.7541823387146</v>
+        <v>124.6163177490234</v>
       </c>
     </row>
     <row r="21">
@@ -652,10 +652,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>264.6406745910645</v>
+        <v>237.3663520812988</v>
       </c>
       <c r="C21" t="n">
-        <v>131.9308090209961</v>
+        <v>123.1806135177612</v>
       </c>
     </row>
     <row r="22">
@@ -663,10 +663,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>266.6907119750977</v>
+        <v>221.2969398498535</v>
       </c>
       <c r="C22" t="n">
-        <v>154.0561723709106</v>
+        <v>121.8217420578003</v>
       </c>
     </row>
     <row r="23">
@@ -674,10 +674,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>283.4620666503906</v>
+        <v>206.0052490234375</v>
       </c>
       <c r="C23" t="n">
-        <v>182.2721099853516</v>
+        <v>124.066801071167</v>
       </c>
     </row>
     <row r="24">
@@ -685,10 +685,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>313.5887908935547</v>
+        <v>194.1226577758789</v>
       </c>
       <c r="C24" t="n">
-        <v>203.6220645904541</v>
+        <v>125.2685308456421</v>
       </c>
     </row>
     <row r="25">
@@ -696,10 +696,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>351.6264343261719</v>
+        <v>184.9114990234375</v>
       </c>
       <c r="C25" t="n">
-        <v>224.6010303497314</v>
+        <v>130.3762722015381</v>
       </c>
     </row>
     <row r="26">
@@ -707,10 +707,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>384.2340469360352</v>
+        <v>178.7818336486816</v>
       </c>
       <c r="C26" t="n">
-        <v>241.2276077270508</v>
+        <v>140.0556564331055</v>
       </c>
     </row>
     <row r="27">
@@ -718,10 +718,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>404.1704559326172</v>
+        <v>176.1171340942383</v>
       </c>
       <c r="C27" t="n">
-        <v>251.5154457092285</v>
+        <v>148.4401702880859</v>
       </c>
     </row>
     <row r="28">
@@ -729,10 +729,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>414.1571807861328</v>
+        <v>176.1407661437988</v>
       </c>
       <c r="C28" t="n">
-        <v>249.6130657196045</v>
+        <v>157.6689577102661</v>
       </c>
     </row>
     <row r="29">
@@ -740,10 +740,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>415.6558990478516</v>
+        <v>180.8287239074707</v>
       </c>
       <c r="C29" t="n">
-        <v>245.6842231750488</v>
+        <v>167.3396301269531</v>
       </c>
     </row>
     <row r="30">
@@ -751,10 +751,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>407.4757385253906</v>
+        <v>187.3880386352539</v>
       </c>
       <c r="C30" t="n">
-        <v>237.5292062759399</v>
+        <v>177.5644254684448</v>
       </c>
     </row>
     <row r="31">
@@ -762,10 +762,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>394.4076538085938</v>
+        <v>198.9091491699219</v>
       </c>
       <c r="C31" t="n">
-        <v>231.8733358383179</v>
+        <v>187.0843505859375</v>
       </c>
     </row>
     <row r="32">
@@ -773,10 +773,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>377.3706817626953</v>
+        <v>211.5151977539062</v>
       </c>
       <c r="C32" t="n">
-        <v>224.3323230743408</v>
+        <v>197.3724746704102</v>
       </c>
     </row>
     <row r="33">
@@ -784,10 +784,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>356.148567199707</v>
+        <v>228.3205032348633</v>
       </c>
       <c r="C33" t="n">
-        <v>218.5560464859009</v>
+        <v>208.0852317810059</v>
       </c>
     </row>
     <row r="34">
@@ -795,10 +795,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>336.1162567138672</v>
+        <v>245.4554557800293</v>
       </c>
       <c r="C34" t="n">
-        <v>209.3081188201904</v>
+        <v>219.0063285827637</v>
       </c>
     </row>
     <row r="35">
@@ -806,10 +806,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>311.1246109008789</v>
+        <v>264.9747276306152</v>
       </c>
       <c r="C35" t="n">
-        <v>214.0882015228271</v>
+        <v>229.1789531707764</v>
       </c>
     </row>
     <row r="36">
@@ -817,10 +817,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>292.4122619628906</v>
+        <v>282.9477882385254</v>
       </c>
       <c r="C36" t="n">
-        <v>226.4350175857544</v>
+        <v>236.1346292495728</v>
       </c>
     </row>
     <row r="37">
@@ -828,10 +828,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>273.5965347290039</v>
+        <v>298.5334205627441</v>
       </c>
       <c r="C37" t="n">
-        <v>232.0559406280518</v>
+        <v>242.3202037811279</v>
       </c>
     </row>
     <row r="38">
@@ -839,10 +839,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>263.2874870300293</v>
+        <v>298.5334205627441</v>
       </c>
       <c r="C38" t="n">
-        <v>243.46604347229</v>
+        <v>242.3202037811279</v>
       </c>
     </row>
     <row r="39">
@@ -850,10 +850,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>253.4922218322754</v>
+        <v>312.2934913635254</v>
       </c>
       <c r="C39" t="n">
-        <v>255.1123809814453</v>
+        <v>245.6957530975342</v>
       </c>
     </row>
     <row r="40">
@@ -861,10 +861,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>258.1885719299316</v>
+        <v>324.3391799926758</v>
       </c>
       <c r="C40" t="n">
-        <v>271.4773178100586</v>
+        <v>248.0888843536377</v>
       </c>
     </row>
     <row r="41">
@@ -872,10 +872,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>438.6212921142578</v>
+        <v>326.2100219726562</v>
       </c>
       <c r="C41" t="n">
-        <v>259.7894096374512</v>
+        <v>248.166675567627</v>
       </c>
     </row>
     <row r="42">
@@ -883,10 +883,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>439.5149993896484</v>
+        <v>323.5784530639648</v>
       </c>
       <c r="C42" t="n">
-        <v>258.8127422332764</v>
+        <v>246.4389324188232</v>
       </c>
     </row>
     <row r="43">
@@ -894,10 +894,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>434.730224609375</v>
+        <v>318.4364700317383</v>
       </c>
       <c r="C43" t="n">
-        <v>274.718713760376</v>
+        <v>246.1782360076904</v>
       </c>
     </row>
     <row r="44">
@@ -905,10 +905,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>414.7475051879883</v>
+        <v>310.3375625610352</v>
       </c>
       <c r="C44" t="n">
-        <v>276.4241409301758</v>
+        <v>245.2166175842285</v>
       </c>
     </row>
     <row r="45">
@@ -916,10 +916,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>410.8992004394531</v>
+        <v>299.0495109558105</v>
       </c>
       <c r="C45" t="n">
-        <v>272.9670238494873</v>
+        <v>242.4559020996094</v>
       </c>
     </row>
     <row r="46">
@@ -927,10 +927,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>422.5400161743164</v>
+        <v>287.0227241516113</v>
       </c>
       <c r="C46" t="n">
-        <v>187.8207635879517</v>
+        <v>240.7041263580322</v>
       </c>
     </row>
     <row r="47">
@@ -938,10 +938,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>435.1999282836914</v>
+        <v>272.3739814758301</v>
       </c>
       <c r="C47" t="n">
-        <v>206.3750553131104</v>
+        <v>240.2332878112793</v>
       </c>
     </row>
     <row r="48">
@@ -949,10 +949,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>447.3643493652344</v>
+        <v>272.3739814758301</v>
       </c>
       <c r="C48" t="n">
-        <v>231.2995147705078</v>
+        <v>240.2332878112793</v>
       </c>
     </row>
     <row r="49">
@@ -960,10 +960,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>460.1935195922852</v>
+        <v>258.166618347168</v>
       </c>
       <c r="C49" t="n">
-        <v>261.3294696807861</v>
+        <v>241.8719673156738</v>
       </c>
     </row>
     <row r="50">
@@ -971,10 +971,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>473.9833831787109</v>
+        <v>243.9486694335938</v>
       </c>
       <c r="C50" t="n">
-        <v>287.0724105834961</v>
+        <v>246.6483306884766</v>
       </c>
     </row>
     <row r="51">
@@ -982,10 +982,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>482.9480361938477</v>
+        <v>229.3948554992676</v>
       </c>
       <c r="C51" t="n">
-        <v>313.0686092376709</v>
+        <v>249.8833465576172</v>
       </c>
     </row>
     <row r="52">
@@ -993,10 +993,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>490.8067321777344</v>
+        <v>209.7288131713867</v>
       </c>
       <c r="C52" t="n">
-        <v>343.0417442321777</v>
+        <v>261.0505485534668</v>
       </c>
     </row>
     <row r="53">
@@ -1004,10 +1004,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>497.4224853515625</v>
+        <v>202.0956611633301</v>
       </c>
       <c r="C53" t="n">
-        <v>362.5098609924316</v>
+        <v>269.9016380310059</v>
       </c>
     </row>
     <row r="54">
@@ -1015,10 +1015,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>502.3526382446289</v>
+        <v>196.9227027893066</v>
       </c>
       <c r="C54" t="n">
-        <v>378.8350582122803</v>
+        <v>277.631950378418</v>
       </c>
     </row>
     <row r="55">
@@ -1026,10 +1026,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>505.0739669799805</v>
+        <v>193.6286163330078</v>
       </c>
       <c r="C55" t="n">
-        <v>386.9590187072754</v>
+        <v>286.9873809814453</v>
       </c>
     </row>
     <row r="56">
@@ -1037,10 +1037,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>505.5512619018555</v>
+        <v>191.7404556274414</v>
       </c>
       <c r="C56" t="n">
-        <v>390.428581237793</v>
+        <v>295.532283782959</v>
       </c>
     </row>
     <row r="57">
@@ -1048,10 +1048,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>503.7461853027344</v>
+        <v>191.7404556274414</v>
       </c>
       <c r="C57" t="n">
-        <v>388.0163669586182</v>
+        <v>295.532283782959</v>
       </c>
     </row>
     <row r="58">
@@ -1059,10 +1059,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>501.7343521118164</v>
+        <v>195.1507568359375</v>
       </c>
       <c r="C58" t="n">
-        <v>384.0595722198486</v>
+        <v>303.2415390014648</v>
       </c>
     </row>
     <row r="59">
@@ -1070,10 +1070,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>498.0921936035156</v>
+        <v>201.2717247009277</v>
       </c>
       <c r="C59" t="n">
-        <v>378.3201313018799</v>
+        <v>310.9980583190918</v>
       </c>
     </row>
     <row r="60">
@@ -1081,10 +1081,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>495.4251480102539</v>
+        <v>211.2743377685547</v>
       </c>
       <c r="C60" t="n">
-        <v>371.3908767700195</v>
+        <v>317.8551578521729</v>
       </c>
     </row>
     <row r="61">
@@ -1092,10 +1092,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>494.2524719238281</v>
+        <v>224.1765594482422</v>
       </c>
       <c r="C61" t="n">
-        <v>365.015230178833</v>
+        <v>326.4860343933105</v>
       </c>
     </row>
     <row r="62">
@@ -1103,10 +1103,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>492.3339080810547</v>
+        <v>237.4317359924316</v>
       </c>
       <c r="C62" t="n">
-        <v>361.9198894500732</v>
+        <v>332.1601295471191</v>
       </c>
     </row>
     <row r="63">
@@ -1114,10 +1114,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>489.3417358398438</v>
+        <v>253.2627487182617</v>
       </c>
       <c r="C63" t="n">
-        <v>360.1632499694824</v>
+        <v>337.410192489624</v>
       </c>
     </row>
     <row r="64">
@@ -1125,10 +1125,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>488.0709838867188</v>
+        <v>288.6498641967773</v>
       </c>
       <c r="C64" t="n">
-        <v>359.436092376709</v>
+        <v>345.6345748901367</v>
       </c>
     </row>
     <row r="65">
@@ -1136,10 +1136,164 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>488.9536285400391</v>
+        <v>304.8026657104492</v>
       </c>
       <c r="C65" t="n">
-        <v>365.6291770935059</v>
+        <v>344.3311214447021</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>304.8026657104492</v>
+      </c>
+      <c r="C66" t="n">
+        <v>344.3311214447021</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>322.8125381469727</v>
+      </c>
+      <c r="C67" t="n">
+        <v>346.3611316680908</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>336.7195129394531</v>
+      </c>
+      <c r="C68" t="n">
+        <v>345.2759456634521</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>351.0630416870117</v>
+      </c>
+      <c r="C69" t="n">
+        <v>347.7375984191895</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>363.4733963012695</v>
+      </c>
+      <c r="C70" t="n">
+        <v>346.0503959655762</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>371.406135559082</v>
+      </c>
+      <c r="C71" t="n">
+        <v>343.9895439147949</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>377.1853637695312</v>
+      </c>
+      <c r="C72" t="n">
+        <v>342.2107315063477</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>380.9870529174805</v>
+      </c>
+      <c r="C73" t="n">
+        <v>340.9621524810791</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>381.7733764648438</v>
+      </c>
+      <c r="C74" t="n">
+        <v>341.1250591278076</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>380.7618713378906</v>
+      </c>
+      <c r="C75" t="n">
+        <v>362.5720882415771</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>375.5272674560547</v>
+      </c>
+      <c r="C76" t="n">
+        <v>388.2195568084717</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>363.931770324707</v>
+      </c>
+      <c r="C77" t="n">
+        <v>400.9485912322998</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="n">
+        <v>360.24658203125</v>
+      </c>
+      <c r="C78" t="n">
+        <v>405.137300491333</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="n">
+        <v>358.3580017089844</v>
+      </c>
+      <c r="C79" t="n">
+        <v>407.5924301147461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated integration code by simpleis6est
</commit_message>
<xml_diff>
--- a/Mergy_Hand_Pose_Estimation_Preprocessing/landmarks.xlsx
+++ b/Mergy_Hand_Pose_Estimation_Preprocessing/landmarks.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,10 +443,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>321.9075393676758</v>
+        <v>301.580696105957</v>
       </c>
       <c r="C2" t="n">
-        <v>156.5245199203491</v>
+        <v>198.6799335479736</v>
       </c>
     </row>
     <row r="3">
@@ -454,10 +454,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>321.1606979370117</v>
+        <v>304.3289184570312</v>
       </c>
       <c r="C3" t="n">
-        <v>156.6767406463623</v>
+        <v>197.5370121002197</v>
       </c>
     </row>
     <row r="4">
@@ -465,10 +465,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>320.3333282470703</v>
+        <v>304.7513389587402</v>
       </c>
       <c r="C4" t="n">
-        <v>156.4820194244385</v>
+        <v>197.4017429351807</v>
       </c>
     </row>
     <row r="5">
@@ -476,10 +476,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>320.5591583251953</v>
+        <v>305.1544570922852</v>
       </c>
       <c r="C5" t="n">
-        <v>157.2189903259277</v>
+        <v>197.4861001968384</v>
       </c>
     </row>
     <row r="6">
@@ -487,10 +487,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>320.1755523681641</v>
+        <v>303.6117172241211</v>
       </c>
       <c r="C6" t="n">
-        <v>157.4060726165771</v>
+        <v>197.1533918380737</v>
       </c>
     </row>
     <row r="7">
@@ -498,10 +498,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>320.0727081298828</v>
+        <v>305.9846687316895</v>
       </c>
       <c r="C7" t="n">
-        <v>157.2195911407471</v>
+        <v>198.3648204803467</v>
       </c>
     </row>
     <row r="8">
@@ -509,10 +509,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>320.9890747070312</v>
+        <v>306.4811706542969</v>
       </c>
       <c r="C8" t="n">
-        <v>157.6928758621216</v>
+        <v>199.904580116272</v>
       </c>
     </row>
     <row r="9">
@@ -520,10 +520,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>322.1222686767578</v>
+        <v>307.416934967041</v>
       </c>
       <c r="C9" t="n">
-        <v>158.0412340164185</v>
+        <v>202.4381446838379</v>
       </c>
     </row>
     <row r="10">
@@ -531,10 +531,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>324.2362976074219</v>
+        <v>310.5128479003906</v>
       </c>
       <c r="C10" t="n">
-        <v>158.3535003662109</v>
+        <v>204.5040035247803</v>
       </c>
     </row>
     <row r="11">
@@ -542,10 +542,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>324.840087890625</v>
+        <v>310.7219886779785</v>
       </c>
       <c r="C11" t="n">
-        <v>157.8266572952271</v>
+        <v>205.3522253036499</v>
       </c>
     </row>
     <row r="12">
@@ -553,10 +553,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>325.7466125488281</v>
+        <v>311.2709808349609</v>
       </c>
       <c r="C12" t="n">
-        <v>157.1883773803711</v>
+        <v>205.8853912353516</v>
       </c>
     </row>
     <row r="13">
@@ -564,10 +564,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>325.0298309326172</v>
+        <v>311.3628387451172</v>
       </c>
       <c r="C13" t="n">
-        <v>156.2177610397339</v>
+        <v>207.3226976394653</v>
       </c>
     </row>
     <row r="14">
@@ -575,10 +575,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>321.9512176513672</v>
+        <v>312.2221946716309</v>
       </c>
       <c r="C14" t="n">
-        <v>154.4462299346924</v>
+        <v>206.9467449188232</v>
       </c>
     </row>
     <row r="15">
@@ -586,10 +586,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>317.0373725891113</v>
+        <v>312.3532104492188</v>
       </c>
       <c r="C15" t="n">
-        <v>149.9756526947021</v>
+        <v>208.0878353118896</v>
       </c>
     </row>
     <row r="16">
@@ -597,10 +597,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>308.841438293457</v>
+        <v>312.8471565246582</v>
       </c>
       <c r="C16" t="n">
-        <v>144.9496078491211</v>
+        <v>208.3736371994019</v>
       </c>
     </row>
     <row r="17">
@@ -608,10 +608,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>296.7984390258789</v>
+        <v>314.3346977233887</v>
       </c>
       <c r="C17" t="n">
-        <v>138.9054107666016</v>
+        <v>209.8037910461426</v>
       </c>
     </row>
     <row r="18">
@@ -619,10 +619,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>283.856201171875</v>
+        <v>316.6686630249023</v>
       </c>
       <c r="C18" t="n">
-        <v>133.2048225402832</v>
+        <v>209.0056085586548</v>
       </c>
     </row>
     <row r="19">
@@ -630,10 +630,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>268.5635757446289</v>
+        <v>317.9023742675781</v>
       </c>
       <c r="C19" t="n">
-        <v>127.4671411514282</v>
+        <v>210.2333736419678</v>
       </c>
     </row>
     <row r="20">
@@ -641,10 +641,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>253.7520217895508</v>
+        <v>324.2375564575195</v>
       </c>
       <c r="C20" t="n">
-        <v>124.6163177490234</v>
+        <v>212.1127080917358</v>
       </c>
     </row>
     <row r="21">
@@ -652,10 +652,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>237.3663520812988</v>
+        <v>324.1802215576172</v>
       </c>
       <c r="C21" t="n">
-        <v>123.1806135177612</v>
+        <v>210.7591581344604</v>
       </c>
     </row>
     <row r="22">
@@ -663,10 +663,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>221.2969398498535</v>
+        <v>314.9545478820801</v>
       </c>
       <c r="C22" t="n">
-        <v>121.8217420578003</v>
+        <v>201.7688941955566</v>
       </c>
     </row>
     <row r="23">
@@ -674,10 +674,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>206.0052490234375</v>
+        <v>295.0443267822266</v>
       </c>
       <c r="C23" t="n">
-        <v>124.066801071167</v>
+        <v>191.7860269546509</v>
       </c>
     </row>
     <row r="24">
@@ -685,10 +685,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>194.1226577758789</v>
+        <v>274.5041656494141</v>
       </c>
       <c r="C24" t="n">
-        <v>125.2685308456421</v>
+        <v>185.2526092529297</v>
       </c>
     </row>
     <row r="25">
@@ -696,10 +696,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>184.9114990234375</v>
+        <v>253.277587890625</v>
       </c>
       <c r="C25" t="n">
-        <v>130.3762722015381</v>
+        <v>185.6079626083374</v>
       </c>
     </row>
     <row r="26">
@@ -707,10 +707,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>178.7818336486816</v>
+        <v>235.5479049682617</v>
       </c>
       <c r="C26" t="n">
-        <v>140.0556564331055</v>
+        <v>209.4093990325928</v>
       </c>
     </row>
     <row r="27">
@@ -718,10 +718,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>176.1171340942383</v>
+        <v>221.2269020080566</v>
       </c>
       <c r="C27" t="n">
-        <v>148.4401702880859</v>
+        <v>208.8348627090454</v>
       </c>
     </row>
     <row r="28">
@@ -729,10 +729,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>176.1407661437988</v>
+        <v>207.7327728271484</v>
       </c>
       <c r="C28" t="n">
-        <v>157.6689577102661</v>
+        <v>210.8592367172241</v>
       </c>
     </row>
     <row r="29">
@@ -740,10 +740,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>180.8287239074707</v>
+        <v>201.8914031982422</v>
       </c>
       <c r="C29" t="n">
-        <v>167.3396301269531</v>
+        <v>218.3521127700806</v>
       </c>
     </row>
     <row r="30">
@@ -751,10 +751,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>187.3880386352539</v>
+        <v>201.1476707458496</v>
       </c>
       <c r="C30" t="n">
-        <v>177.5644254684448</v>
+        <v>228.155779838562</v>
       </c>
     </row>
     <row r="31">
@@ -762,10 +762,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>198.9091491699219</v>
+        <v>205.6510543823242</v>
       </c>
       <c r="C31" t="n">
-        <v>187.0843505859375</v>
+        <v>240.5823612213135</v>
       </c>
     </row>
     <row r="32">
@@ -773,10 +773,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>211.5151977539062</v>
+        <v>212.9120063781738</v>
       </c>
       <c r="C32" t="n">
-        <v>197.3724746704102</v>
+        <v>249.8719596862793</v>
       </c>
     </row>
     <row r="33">
@@ -784,10 +784,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>228.3205032348633</v>
+        <v>222.310791015625</v>
       </c>
       <c r="C33" t="n">
-        <v>208.0852317810059</v>
+        <v>258.7912845611572</v>
       </c>
     </row>
     <row r="34">
@@ -795,10 +795,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>245.4554557800293</v>
+        <v>228.3261108398438</v>
       </c>
       <c r="C34" t="n">
-        <v>219.0063285827637</v>
+        <v>264.5145606994629</v>
       </c>
     </row>
     <row r="35">
@@ -806,10 +806,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>264.9747276306152</v>
+        <v>243.9634704589844</v>
       </c>
       <c r="C35" t="n">
-        <v>229.1789531707764</v>
+        <v>273.3255386352539</v>
       </c>
     </row>
     <row r="36">
@@ -817,10 +817,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>282.9477882385254</v>
+        <v>295.644359588623</v>
       </c>
       <c r="C36" t="n">
-        <v>236.1346292495728</v>
+        <v>290.8289051055908</v>
       </c>
     </row>
     <row r="37">
@@ -828,10 +828,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>298.5334205627441</v>
+        <v>317.238712310791</v>
       </c>
       <c r="C37" t="n">
-        <v>242.3202037811279</v>
+        <v>293.3724117279053</v>
       </c>
     </row>
     <row r="38">
@@ -839,10 +839,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>298.5334205627441</v>
+        <v>337.2767639160156</v>
       </c>
       <c r="C38" t="n">
-        <v>242.3202037811279</v>
+        <v>301.2234020233154</v>
       </c>
     </row>
     <row r="39">
@@ -850,10 +850,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>312.2934913635254</v>
+        <v>336.4676284790039</v>
       </c>
       <c r="C39" t="n">
-        <v>245.6957530975342</v>
+        <v>383.2715892791748</v>
       </c>
     </row>
     <row r="40">
@@ -861,10 +861,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>324.3391799926758</v>
+        <v>344.6207427978516</v>
       </c>
       <c r="C40" t="n">
-        <v>248.0888843536377</v>
+        <v>389.3365287780762</v>
       </c>
     </row>
     <row r="41">
@@ -872,10 +872,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>326.2100219726562</v>
+        <v>362.9837799072266</v>
       </c>
       <c r="C41" t="n">
-        <v>248.166675567627</v>
+        <v>307.8590297698975</v>
       </c>
     </row>
     <row r="42">
@@ -883,10 +883,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>323.5784530639648</v>
+        <v>347.883186340332</v>
       </c>
       <c r="C42" t="n">
-        <v>246.4389324188232</v>
+        <v>348.1959915161133</v>
       </c>
     </row>
     <row r="43">
@@ -894,10 +894,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>318.4364700317383</v>
+        <v>368.4585189819336</v>
       </c>
       <c r="C43" t="n">
-        <v>246.1782360076904</v>
+        <v>306.1020755767822</v>
       </c>
     </row>
     <row r="44">
@@ -905,10 +905,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>310.3375625610352</v>
+        <v>367.7604293823242</v>
       </c>
       <c r="C44" t="n">
-        <v>245.2166175842285</v>
+        <v>306.2249851226807</v>
       </c>
     </row>
     <row r="45">
@@ -916,10 +916,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>299.0495109558105</v>
+        <v>364.7008895874023</v>
       </c>
       <c r="C45" t="n">
-        <v>242.4559020996094</v>
+        <v>307.5014305114746</v>
       </c>
     </row>
     <row r="46">
@@ -927,10 +927,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>287.0227241516113</v>
+        <v>364.1349792480469</v>
       </c>
       <c r="C46" t="n">
-        <v>240.7041263580322</v>
+        <v>309.1973876953125</v>
       </c>
     </row>
     <row r="47">
@@ -938,10 +938,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>272.3739814758301</v>
+        <v>361.223258972168</v>
       </c>
       <c r="C47" t="n">
-        <v>240.2332878112793</v>
+        <v>306.9017887115479</v>
       </c>
     </row>
     <row r="48">
@@ -949,10 +949,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>272.3739814758301</v>
+        <v>357.4379730224609</v>
       </c>
       <c r="C48" t="n">
-        <v>240.2332878112793</v>
+        <v>306.8339538574219</v>
       </c>
     </row>
     <row r="49">
@@ -960,10 +960,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>258.166618347168</v>
+        <v>357.2548294067383</v>
       </c>
       <c r="C49" t="n">
-        <v>241.8719673156738</v>
+        <v>305.3340339660645</v>
       </c>
     </row>
     <row r="50">
@@ -971,10 +971,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>243.9486694335938</v>
+        <v>338.4324645996094</v>
       </c>
       <c r="C50" t="n">
-        <v>246.6483306884766</v>
+        <v>336.7652893066406</v>
       </c>
     </row>
     <row r="51">
@@ -982,10 +982,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>229.3948554992676</v>
+        <v>356.0394287109375</v>
       </c>
       <c r="C51" t="n">
-        <v>249.8833465576172</v>
+        <v>304.2288780212402</v>
       </c>
     </row>
     <row r="52">
@@ -993,10 +993,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>209.7288131713867</v>
+        <v>356.7615509033203</v>
       </c>
       <c r="C52" t="n">
-        <v>261.0505485534668</v>
+        <v>303.0307960510254</v>
       </c>
     </row>
     <row r="53">
@@ -1004,10 +1004,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>202.0956611633301</v>
+        <v>320.1678848266602</v>
       </c>
       <c r="C53" t="n">
-        <v>269.9016380310059</v>
+        <v>393.3853912353516</v>
       </c>
     </row>
     <row r="54">
@@ -1015,10 +1015,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>196.9227027893066</v>
+        <v>356.8764495849609</v>
       </c>
       <c r="C54" t="n">
-        <v>277.631950378418</v>
+        <v>303.7191581726074</v>
       </c>
     </row>
     <row r="55">
@@ -1026,10 +1026,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>193.6286163330078</v>
+        <v>356.8891906738281</v>
       </c>
       <c r="C55" t="n">
-        <v>286.9873809814453</v>
+        <v>302.2235584259033</v>
       </c>
     </row>
     <row r="56">
@@ -1037,10 +1037,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>191.7404556274414</v>
+        <v>355.1534652709961</v>
       </c>
       <c r="C56" t="n">
-        <v>295.532283782959</v>
+        <v>304.0714931488037</v>
       </c>
     </row>
     <row r="57">
@@ -1048,10 +1048,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>191.7404556274414</v>
+        <v>354.8737716674805</v>
       </c>
       <c r="C57" t="n">
-        <v>295.532283782959</v>
+        <v>303.988151550293</v>
       </c>
     </row>
     <row r="58">
@@ -1059,10 +1059,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>195.1507568359375</v>
+        <v>355.010871887207</v>
       </c>
       <c r="C58" t="n">
-        <v>303.2415390014648</v>
+        <v>304.6842098236084</v>
       </c>
     </row>
     <row r="59">
@@ -1070,10 +1070,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>201.2717247009277</v>
+        <v>353.9480590820312</v>
       </c>
       <c r="C59" t="n">
-        <v>310.9980583190918</v>
+        <v>303.4764862060547</v>
       </c>
     </row>
     <row r="60">
@@ -1081,10 +1081,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>211.2743377685547</v>
+        <v>350.3170394897461</v>
       </c>
       <c r="C60" t="n">
-        <v>317.8551578521729</v>
+        <v>302.4907779693604</v>
       </c>
     </row>
     <row r="61">
@@ -1092,10 +1092,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>224.1765594482422</v>
+        <v>347.1619415283203</v>
       </c>
       <c r="C61" t="n">
-        <v>326.4860343933105</v>
+        <v>300.0793075561523</v>
       </c>
     </row>
     <row r="62">
@@ -1103,10 +1103,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>237.4317359924316</v>
+        <v>340.5611419677734</v>
       </c>
       <c r="C62" t="n">
-        <v>332.1601295471191</v>
+        <v>295.01051902771</v>
       </c>
     </row>
     <row r="63">
@@ -1114,10 +1114,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>253.2627487182617</v>
+        <v>333.5683822631836</v>
       </c>
       <c r="C63" t="n">
-        <v>337.410192489624</v>
+        <v>293.0414199829102</v>
       </c>
     </row>
     <row r="64">
@@ -1125,10 +1125,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>288.6498641967773</v>
+        <v>321.9160461425781</v>
       </c>
       <c r="C64" t="n">
-        <v>345.6345748901367</v>
+        <v>288.7927722930908</v>
       </c>
     </row>
     <row r="65">
@@ -1136,10 +1136,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>304.8026657104492</v>
+        <v>307.404670715332</v>
       </c>
       <c r="C65" t="n">
-        <v>344.3311214447021</v>
+        <v>286.391429901123</v>
       </c>
     </row>
     <row r="66">
@@ -1147,10 +1147,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>304.8026657104492</v>
+        <v>293.4063529968262</v>
       </c>
       <c r="C66" t="n">
-        <v>344.3311214447021</v>
+        <v>285.0151920318604</v>
       </c>
     </row>
     <row r="67">
@@ -1158,10 +1158,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>322.8125381469727</v>
+        <v>277.347297668457</v>
       </c>
       <c r="C67" t="n">
-        <v>346.3611316680908</v>
+        <v>286.5023517608643</v>
       </c>
     </row>
     <row r="68">
@@ -1169,10 +1169,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>336.7195129394531</v>
+        <v>254.8833465576172</v>
       </c>
       <c r="C68" t="n">
-        <v>345.2759456634521</v>
+        <v>299.1382026672363</v>
       </c>
     </row>
     <row r="69">
@@ -1180,10 +1180,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>351.0630416870117</v>
+        <v>240.1508712768555</v>
       </c>
       <c r="C69" t="n">
-        <v>347.7375984191895</v>
+        <v>309.7138595581055</v>
       </c>
     </row>
     <row r="70">
@@ -1191,10 +1191,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>363.4733963012695</v>
+        <v>231.8825912475586</v>
       </c>
       <c r="C70" t="n">
-        <v>346.0503959655762</v>
+        <v>311.5981006622314</v>
       </c>
     </row>
     <row r="71">
@@ -1202,10 +1202,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>371.406135559082</v>
+        <v>221.7786407470703</v>
       </c>
       <c r="C71" t="n">
-        <v>343.9895439147949</v>
+        <v>319.5260810852051</v>
       </c>
     </row>
     <row r="72">
@@ -1213,10 +1213,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>377.1853637695312</v>
+        <v>213.0893516540527</v>
       </c>
       <c r="C72" t="n">
-        <v>342.2107315063477</v>
+        <v>328.7232112884521</v>
       </c>
     </row>
     <row r="73">
@@ -1224,10 +1224,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>380.9870529174805</v>
+        <v>209.624137878418</v>
       </c>
       <c r="C73" t="n">
-        <v>340.9621524810791</v>
+        <v>341.1438274383545</v>
       </c>
     </row>
     <row r="74">
@@ -1235,10 +1235,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>381.7733764648438</v>
+        <v>256.7561149597168</v>
       </c>
       <c r="C74" t="n">
-        <v>341.1250591278076</v>
+        <v>493.2778358459473</v>
       </c>
     </row>
     <row r="75">
@@ -1246,10 +1246,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>380.7618713378906</v>
+        <v>332.5244903564453</v>
       </c>
       <c r="C75" t="n">
-        <v>362.5720882415771</v>
+        <v>478.2175540924072</v>
       </c>
     </row>
     <row r="76">
@@ -1257,10 +1257,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>375.5272674560547</v>
+        <v>362.150993347168</v>
       </c>
       <c r="C76" t="n">
-        <v>388.2195568084717</v>
+        <v>480.5669403076172</v>
       </c>
     </row>
     <row r="77">
@@ -1268,10 +1268,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>363.931770324707</v>
+        <v>365.5131149291992</v>
       </c>
       <c r="C77" t="n">
-        <v>400.9485912322998</v>
+        <v>482.5569534301758</v>
       </c>
     </row>
     <row r="78">
@@ -1279,10 +1279,10 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>360.24658203125</v>
+        <v>401.2774276733398</v>
       </c>
       <c r="C78" t="n">
-        <v>405.137300491333</v>
+        <v>392.2531414031982</v>
       </c>
     </row>
     <row r="79">
@@ -1290,10 +1290,384 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>358.3580017089844</v>
+        <v>406.2438583374023</v>
       </c>
       <c r="C79" t="n">
-        <v>407.5924301147461</v>
+        <v>388.3743667602539</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="n">
+        <v>409.8681640625</v>
+      </c>
+      <c r="C80" t="n">
+        <v>384.2517185211182</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="n">
+        <v>413.0849838256836</v>
+      </c>
+      <c r="C81" t="n">
+        <v>383.8685703277588</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="n">
+        <v>416.4176940917969</v>
+      </c>
+      <c r="C82" t="n">
+        <v>377.2506237030029</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="n">
+        <v>420.0083160400391</v>
+      </c>
+      <c r="C83" t="n">
+        <v>375.6314849853516</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="n">
+        <v>421.7411804199219</v>
+      </c>
+      <c r="C84" t="n">
+        <v>371.123514175415</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="n">
+        <v>422.6917266845703</v>
+      </c>
+      <c r="C85" t="n">
+        <v>371.2782096862793</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="n">
+        <v>422.4713897705078</v>
+      </c>
+      <c r="C86" t="n">
+        <v>371.1333847045898</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="n">
+        <v>420.1962280273438</v>
+      </c>
+      <c r="C87" t="n">
+        <v>373.1639671325684</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="n">
+        <v>418.6752319335938</v>
+      </c>
+      <c r="C88" t="n">
+        <v>372.9774856567383</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="n">
+        <v>417.9193496704102</v>
+      </c>
+      <c r="C89" t="n">
+        <v>373.9857959747314</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="n">
+        <v>418.8997650146484</v>
+      </c>
+      <c r="C90" t="n">
+        <v>373.7307357788086</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="n">
+        <v>417.7945709228516</v>
+      </c>
+      <c r="C91" t="n">
+        <v>374.33349609375</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="n">
+        <v>417.6186370849609</v>
+      </c>
+      <c r="C92" t="n">
+        <v>376.0244464874268</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="n">
+        <v>416.9873809814453</v>
+      </c>
+      <c r="C93" t="n">
+        <v>375.0797080993652</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="n">
+        <v>417.0002746582031</v>
+      </c>
+      <c r="C94" t="n">
+        <v>373.7006950378418</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="n">
+        <v>418.6467742919922</v>
+      </c>
+      <c r="C95" t="n">
+        <v>373.7280750274658</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="n">
+        <v>418.184700012207</v>
+      </c>
+      <c r="C96" t="n">
+        <v>373.2118606567383</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="n">
+        <v>418.8584518432617</v>
+      </c>
+      <c r="C97" t="n">
+        <v>371.608772277832</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="n">
+        <v>416.9054412841797</v>
+      </c>
+      <c r="C98" t="n">
+        <v>368.3235740661621</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="n">
+        <v>412.9043960571289</v>
+      </c>
+      <c r="C99" t="n">
+        <v>362.9985237121582</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="n">
+        <v>405.9521102905273</v>
+      </c>
+      <c r="C100" t="n">
+        <v>350.3407287597656</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="n">
+        <v>404.2134857177734</v>
+      </c>
+      <c r="C101" t="n">
+        <v>343.0961894989014</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="n">
+        <v>396.3188934326172</v>
+      </c>
+      <c r="C102" t="n">
+        <v>332.9078578948975</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="n">
+        <v>391.0876846313477</v>
+      </c>
+      <c r="C103" t="n">
+        <v>324.2669677734375</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="n">
+        <v>390.6815338134766</v>
+      </c>
+      <c r="C104" t="n">
+        <v>318.4580039978027</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="n">
+        <v>384.7146987915039</v>
+      </c>
+      <c r="C105" t="n">
+        <v>308.1191253662109</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="n">
+        <v>381.8271255493164</v>
+      </c>
+      <c r="C106" t="n">
+        <v>296.0513591766357</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="n">
+        <v>380.3066635131836</v>
+      </c>
+      <c r="C107" t="n">
+        <v>289.9652767181396</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="n">
+        <v>375.214729309082</v>
+      </c>
+      <c r="C108" t="n">
+        <v>282.5899028778076</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="n">
+        <v>374.1634368896484</v>
+      </c>
+      <c r="C109" t="n">
+        <v>292.9549884796143</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="n">
+        <v>343.3008193969727</v>
+      </c>
+      <c r="C110" t="n">
+        <v>349.8074054718018</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="n">
+        <v>339.8038101196289</v>
+      </c>
+      <c r="C111" t="n">
+        <v>344.6346473693848</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="n">
+        <v>337.8397750854492</v>
+      </c>
+      <c r="C112" t="n">
+        <v>360.8515548706055</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="n">
+        <v>334.2683029174805</v>
+      </c>
+      <c r="C113" t="n">
+        <v>364.176778793335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>